<commit_message>
Updated lang info for lll-livgf055 per #49
</commit_message>
<xml_diff>
--- a/processed_data/participants_cleaned/LLL_Liv_Participants.xlsx
+++ b/processed_data/participants_cleaned/LLL_Liv_Participants.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5360" yWindow="9300" windowWidth="34720" windowHeight="16820"/>
+    <workbookView xWindow="16380" yWindow="8580" windowWidth="34720" windowHeight="16820"/>
   </bookViews>
   <sheets>
     <sheet name="Combined" sheetId="7" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3345" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3345" uniqueCount="234">
   <si>
     <t>method</t>
   </si>
@@ -622,9 +622,6 @@
   </si>
   <si>
     <t xml:space="preserve">Japanese </t>
-  </si>
-  <si>
-    <t>Japanese</t>
   </si>
   <si>
     <t xml:space="preserve">French </t>
@@ -1172,7 +1169,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1182,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="AT15" sqref="AT15"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="N66" sqref="N66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1250,10 +1247,10 @@
         <v>15</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>96</v>
@@ -1283,7 +1280,7 @@
         <v>22</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AG1" s="1" t="s">
         <v>23</v>
@@ -2105,7 +2102,7 @@
         <v>168</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>111</v>
@@ -2638,7 +2635,7 @@
         <v>168</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>111</v>
@@ -2817,7 +2814,7 @@
         <v>168</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>111</v>
@@ -3175,7 +3172,7 @@
         <v>168</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>111</v>
@@ -3354,7 +3351,7 @@
         <v>168</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>111</v>
@@ -3533,7 +3530,7 @@
         <v>168</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>111</v>
@@ -8692,7 +8689,7 @@
         <v>87</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J43" s="3" t="s">
         <v>111</v>
@@ -9566,7 +9563,7 @@
         <v>85</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>26</v>
@@ -9587,13 +9584,13 @@
         <v>87</v>
       </c>
       <c r="I48" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J48" s="16" t="s">
         <v>111</v>
       </c>
       <c r="K48" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L48" t="s">
         <v>63</v>
@@ -9739,7 +9736,7 @@
         <v>85</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>26</v>
@@ -9764,7 +9761,7 @@
         <v>111</v>
       </c>
       <c r="K49" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L49" t="s">
         <v>30</v>
@@ -9910,7 +9907,7 @@
         <v>85</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>26</v>
@@ -9931,13 +9928,13 @@
         <v>178</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J50" s="16" t="s">
         <v>111</v>
       </c>
       <c r="K50" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L50" t="s">
         <v>30</v>
@@ -10083,7 +10080,7 @@
         <v>85</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>26</v>
@@ -10108,7 +10105,7 @@
         <v>111</v>
       </c>
       <c r="K51" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L51" t="s">
         <v>67</v>
@@ -10254,7 +10251,7 @@
         <v>85</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>26</v>
@@ -10275,13 +10272,13 @@
         <v>87</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J52" s="16" t="s">
         <v>111</v>
       </c>
       <c r="K52" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L52" t="s">
         <v>60</v>
@@ -10427,7 +10424,7 @@
         <v>85</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>26</v>
@@ -10452,7 +10449,7 @@
         <v>111</v>
       </c>
       <c r="K53" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L53" t="s">
         <v>30</v>
@@ -10598,7 +10595,7 @@
         <v>85</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>26</v>
@@ -10623,7 +10620,7 @@
         <v>111</v>
       </c>
       <c r="K54" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L54" t="s">
         <v>30</v>
@@ -10769,7 +10766,7 @@
         <v>85</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>26</v>
@@ -10790,13 +10787,13 @@
         <v>87</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J55" s="16" t="s">
         <v>111</v>
       </c>
       <c r="K55" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L55" t="s">
         <v>60</v>
@@ -10942,7 +10939,7 @@
         <v>85</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>26</v>
@@ -10967,7 +10964,7 @@
         <v>111</v>
       </c>
       <c r="K56" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L56" t="s">
         <v>30</v>
@@ -11113,7 +11110,7 @@
         <v>85</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>26</v>
@@ -11138,7 +11135,7 @@
         <v>111</v>
       </c>
       <c r="K57" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L57" t="s">
         <v>30</v>
@@ -11284,7 +11281,7 @@
         <v>85</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>26</v>
@@ -11309,7 +11306,7 @@
         <v>111</v>
       </c>
       <c r="K58" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L58" t="s">
         <v>35</v>
@@ -11455,7 +11452,7 @@
         <v>85</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>26</v>
@@ -11476,13 +11473,13 @@
         <v>87</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J59" s="16" t="s">
         <v>111</v>
       </c>
       <c r="K59" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L59" t="s">
         <v>190</v>
@@ -11628,7 +11625,7 @@
         <v>85</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>26</v>
@@ -11655,7 +11652,7 @@
         <v>111</v>
       </c>
       <c r="K60" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L60" t="s">
         <v>193</v>
@@ -11801,7 +11798,7 @@
         <v>85</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>26</v>
@@ -11826,7 +11823,7 @@
         <v>111</v>
       </c>
       <c r="K61" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L61" t="s">
         <v>30</v>
@@ -11972,7 +11969,7 @@
         <v>85</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>26</v>
@@ -11997,7 +11994,7 @@
         <v>111</v>
       </c>
       <c r="K62" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L62" t="s">
         <v>179</v>
@@ -12143,7 +12140,7 @@
         <v>85</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>26</v>
@@ -12168,7 +12165,7 @@
         <v>111</v>
       </c>
       <c r="K63" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L63" t="s">
         <v>30</v>
@@ -12314,7 +12311,7 @@
         <v>85</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>26</v>
@@ -12335,13 +12332,13 @@
         <v>87</v>
       </c>
       <c r="I64" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J64" s="16" t="s">
         <v>111</v>
       </c>
       <c r="K64" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L64" t="s">
         <v>199</v>
@@ -12487,7 +12484,7 @@
         <v>85</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>26</v>
@@ -12512,7 +12509,7 @@
         <v>111</v>
       </c>
       <c r="K65" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L65" t="s">
         <v>199</v>
@@ -12521,13 +12518,13 @@
         <v>74.900000000000006</v>
       </c>
       <c r="N65" s="19" t="s">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="O65" s="19">
         <v>25.1</v>
       </c>
       <c r="P65" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="Q65" t="s">
         <v>87</v>
@@ -12658,7 +12655,7 @@
         <v>85</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>26</v>
@@ -12683,7 +12680,7 @@
         <v>111</v>
       </c>
       <c r="K66" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L66" t="s">
         <v>30</v>
@@ -12692,7 +12689,7 @@
         <v>81.5</v>
       </c>
       <c r="N66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O66">
         <v>18.5</v>
@@ -12815,7 +12812,7 @@
         <v>56</v>
       </c>
       <c r="BC66" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="BD66" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
lll-liv gf015 and gf045 were fussy and had no data beyond attention getters.  Updated participant and no data sheets. Per #56
</commit_message>
<xml_diff>
--- a/processed_data/participants_cleaned/LLL_Liv_Participants.xlsx
+++ b/processed_data/participants_cleaned/LLL_Liv_Participants.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3345" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3345" uniqueCount="235">
   <si>
     <t>method</t>
   </si>
@@ -724,6 +724,9 @@
   </si>
   <si>
     <t>hearing_vision</t>
+  </si>
+  <si>
+    <t>fussy</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1172,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1179,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="N66" sqref="N66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3880,10 +3883,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>87</v>
+        <v>234</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3" t="s">
@@ -6372,10 +6375,10 @@
         <v>1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>87</v>
+        <v>234</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>161</v>

</xml_diff>